<commit_message>
Explain steps to load the OS and prepare the pinout for the weather station (in progress)
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jlaffosse\Documents\Perso\Weather Station\weather_station\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E70789F-1809-4F4D-94D3-9B3F142DAA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DB2785-C27C-4848-8361-0317595EC85F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Date:</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Adafruit Link</t>
   </si>
   <si>
-    <t>Unit Price (CAD)</t>
-  </si>
-  <si>
     <t>AHT20</t>
   </si>
   <si>
@@ -138,7 +135,61 @@
     <t>Adafruit</t>
   </si>
   <si>
-    <t>Total (CAD)</t>
+    <t>Raspberry Case</t>
+  </si>
+  <si>
+    <t>Official Raspberry Pi Foundation Raspberry Pi 4 Case - Red White</t>
+  </si>
+  <si>
+    <t>Power supply</t>
+  </si>
+  <si>
+    <t>Official Raspberry Pi Power Supply 5.1V 3A with USB C - 1.5 meter long</t>
+  </si>
+  <si>
+    <t>Micro B USB to USB C Adapter</t>
+  </si>
+  <si>
+    <t>16GB Card with NOOBS 3.1 for Raspberry Pi Computers including 4</t>
+  </si>
+  <si>
+    <t>Micro SD card</t>
+  </si>
+  <si>
+    <t>Micro-HDMI to HDMI Cable</t>
+  </si>
+  <si>
+    <t>Micro HDMI to HDMI Cable - 2 meter</t>
+  </si>
+  <si>
+    <t>Fan and Heatsink + Case</t>
+  </si>
+  <si>
+    <t>Official Raspberry Pi 4 Case Fan and Heatsink</t>
+  </si>
+  <si>
+    <t>STEMMA QT / Qwiic JST SH 4-pin Cable with Premium Female Sockets - 150mm Long</t>
+  </si>
+  <si>
+    <t>Cables Adapter</t>
+  </si>
+  <si>
+    <t>Cables extension</t>
+  </si>
+  <si>
+    <t>STEMMA QT / Qwiic JST SH 4-pin Cable - 100mm Long</t>
+  </si>
+  <si>
+    <t>Unit Price (USD)</t>
+  </si>
+  <si>
+    <t>Total (USD)</t>
+  </si>
+  <si>
+    <t>Not used for the weather station</t>
+  </si>
+  <si>
+    <t>TBD if 2 cables are needed</t>
   </si>
 </sst>
 </file>
@@ -300,7 +351,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -323,10 +374,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -353,12 +404,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,6 +412,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -654,21 +702,21 @@
   <dimension ref="B1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="2"/>
+    <col min="1" max="2" width="9.109375" style="2"/>
     <col min="3" max="3" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="9.109375" style="2"/>
+    <col min="5" max="5" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
@@ -676,7 +724,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
         <v>0</v>
       </c>
@@ -684,7 +732,7 @@
         <v>45518</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
@@ -692,8 +740,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14" t="s">
         <v>5</v>
       </c>
@@ -710,7 +758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
@@ -727,42 +775,42 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -776,28 +824,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB770D36-0313-4D34-8F36-6C085DF1C7E1}">
-  <dimension ref="B1:J12"/>
+  <dimension ref="B1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
     <col min="2" max="2" width="52" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="53.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="18" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13" style="18" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="27.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="53.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="8" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="14" t="s">
         <v>13</v>
       </c>
@@ -814,36 +862,36 @@
         <v>17</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>15</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>29</v>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H3" s="8">
         <v>55</v>
@@ -851,29 +899,29 @@
       <c r="I3" s="8">
         <v>1</v>
       </c>
-      <c r="J3" s="21">
+      <c r="J3" s="19">
         <f>H3*I3</f>
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="19" t="s">
-        <v>28</v>
+      <c r="F4" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="8">
         <v>4.5</v>
@@ -881,29 +929,29 @@
       <c r="I4" s="8">
         <v>1</v>
       </c>
-      <c r="J4" s="21">
-        <f t="shared" ref="J4:J5" si="0">H4*I4</f>
+      <c r="J4" s="19">
+        <f t="shared" ref="J4:J16" si="0">H4*I4</f>
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>28</v>
-      </c>
       <c r="G5" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="8">
         <v>6.95</v>
@@ -911,93 +959,275 @@
       <c r="I5" s="8">
         <v>1</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="19">
         <f t="shared" si="0"/>
         <v>6.95</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="21"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="21"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="21"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="21"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="21"/>
-    </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="6"/>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1322</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="8">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
+      <c r="J6" s="19">
+        <f t="shared" si="0"/>
+        <v>8.9499999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4301</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="8">
+        <v>6</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1</v>
+      </c>
+      <c r="J7" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4298</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="8">
+        <v>7.95</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="19">
+        <f t="shared" si="0"/>
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4299</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1.25</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="8">
+        <v>4266</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="8">
+        <v>14.95</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1</v>
+      </c>
+      <c r="J10" s="19">
+        <f t="shared" si="0"/>
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="8">
+        <v>4794</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="8">
+        <v>5</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="19">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="8">
+        <v>4397</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="I12" s="8">
+        <v>2</v>
+      </c>
+      <c r="J12" s="19">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="8">
+        <v>4210</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="I13" s="8">
+        <v>1</v>
+      </c>
+      <c r="J13" s="19">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="3"/>
+      <c r="E14" s="21"/>
+      <c r="J14" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="3"/>
+      <c r="J15" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="5"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{3EA2D7ED-C13E-4DD5-BAD4-3754DB1795E5}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{9A01B44B-76A3-4412-8231-41834604A7F8}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{69EAE364-21A6-486D-9E0E-0CB9F3084CEA}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{C2EAB49A-A7F6-4D6D-B2FE-CF9AA335DA46}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{9147224C-156D-4966-ADD2-E4864D5748B0}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{5D7F9425-25BD-40F8-8BD9-D1F80D19B449}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{3B2D81EC-D493-49DA-B1DB-87C9B415A5B4}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{67744DE0-7D8F-4946-9AEB-D04206B987B2}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{9C28C8D7-E069-414C-B6D6-BBD1464F33A3}"/>
+    <hyperlink ref="E12" r:id="rId10" xr:uid="{BE28C9B9-1D53-4CF6-8B20-41E50B8C1C64}"/>
+    <hyperlink ref="E13" r:id="rId11" xr:uid="{716A421A-FF18-4D76-A04C-06662898B8A0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>